<commit_message>
Changes done and Excel updated
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\All Coding Stuff\Spring-Boot_Journey\Udemy_project\Dennis\InventoryManagementSystem\InventoryManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181B68F5-9429-45D3-8151-CAA7EDAC7A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95407C9A-2544-44AE-BF16-703109A9FDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -34,13 +34,25 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Writtern required Entities</t>
+  </si>
+  <si>
+    <t>Categories, Product, User, Supplier, Transactions</t>
+  </si>
+  <si>
+    <t>T0-DO</t>
+  </si>
+  <si>
+    <t>DTO,Create Repositories,Exceptions,Auth Users, Customer User Details,JWT Utils ,Auth Filter,SecurityFIlter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +60,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -65,14 +90,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,28 +406,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45877</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45878</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45879</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45884</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45885</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45886</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45887</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45889</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45890</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45892</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45893</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45895</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45898</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All security files configured and updated.
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\All Coding Stuff\Spring-Boot_Journey\Udemy_project\Dennis\InventoryManagementSystem\InventoryManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB30EFE-2787-41FF-B5F9-052E8F93391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B436703-3AD0-4779-A298-C27BBC820F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -42,26 +42,77 @@
     <t>Categories, Product, User, Supplier, Transactions</t>
   </si>
   <si>
-    <t>T0-DO</t>
-  </si>
-  <si>
-    <t>DTO,Create Repositories</t>
-  </si>
-  <si>
-    <t>,Exceptions,Auth Users, Customer User Details,JWT Utils ,Auth Filter,SecurityFIlter</t>
-  </si>
-  <si>
     <t xml:space="preserve">Done DTO and repo </t>
   </si>
   <si>
     <t>DTO for Encaps, and repo for search functionality</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Exceptions,Auth Users, Customer User Details,JWT Utils ,Auth Filter,Security FIlter</t>
+  </si>
+  <si>
+    <t>Specification Filter and user Service , Controller and test</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Category Service, Controller and text | Supplier Service , controller&amp;Test | Product service controller and test</t>
+  </si>
+  <si>
+    <t>Transaction service controller and test  + Back Log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All security files configured. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front end : Create Project , service layout and pagination +  Frontend Auth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontend : Admin Management Pages </t>
+  </si>
+  <si>
+    <t>Front-End Manager's Page (Purchase , sales , transaction)</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> revising all backend code .</t>
+  </si>
+  <si>
+    <t>DashBoard pages and Profile Pages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,8 +128,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,11 +159,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -123,16 +226,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -141,6 +280,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA9D08E"/>
+      <color rgb="FFFC7A64"/>
+      <color rgb="FFFC4936"/>
+      <color rgb="FF99FF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,174 +562,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="79.88671875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="84.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <v>45877</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45878</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>45877</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>45878</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45879</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45880</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4">
+        <v>45881</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45882</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>45879</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>45880</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>45881</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>45882</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    </row>
+    <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4">
         <v>45883</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4">
         <v>45884</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4">
         <v>45885</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
         <v>45886</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4">
         <v>45887</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
         <v>45888</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
         <v>45889</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="C14" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
         <v>45890</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
         <v>45891</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
         <v>45892</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
         <v>45893</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
         <v>45894</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4">
         <v>45895</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="4">
         <v>45896</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
         <v>45897</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="4">
         <v>45898</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4">
         <v>45899</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
         <v>45900</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User Services implemented and ran successfully
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\All Coding Stuff\Spring-Boot_Journey\Udemy_project\Dennis\InventoryManagementSystem\InventoryManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B436703-3AD0-4779-A298-C27BBC820F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAB1A4D-1F0E-4C83-BDE9-8EF76C400E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -670,9 +670,7 @@
       <c r="B7" s="4">
         <v>45882</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -682,7 +680,7 @@
         <v>45883</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -693,7 +691,7 @@
         <v>45884</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -704,7 +702,7 @@
         <v>45885</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -715,7 +713,7 @@
         <v>45886</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>24</v>
@@ -729,7 +727,7 @@
         <v>45887</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -740,7 +738,7 @@
         <v>45888</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -762,7 +760,7 @@
         <v>45890</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -773,18 +771,21 @@
         <v>45891</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4">
         <v>45892</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -792,7 +793,7 @@
         <v>45893</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -800,7 +801,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -808,27 +809,27 @@
         <v>45895</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <v>45896</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>45897</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>45898</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <v>45899</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>45900</v>
       </c>

</xml_diff>

<commit_message>
Completed and Tested Category, Supplier and Product services. Excel Updated
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\All Coding Stuff\Spring-Boot_Journey\Udemy_project\Dennis\InventoryManagementSystem\InventoryManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88E7F79-5457-4C41-8855-D3BB0AD0AE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992EAB1-F33C-4E83-A71B-3CCF1600D87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Implemented the user service functionality and tested API accordingly</t>
+  </si>
+  <si>
+    <t>Implemented the category service , supplier service and Product service</t>
   </si>
 </sst>
 </file>
@@ -576,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -728,8 +731,14 @@
       <c r="B9" s="4">
         <v>45884</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>